<commit_message>
Major content update species, freshwater, estuaries, marine - package updated but no freezer off build
</commit_message>
<xml_diff>
--- a/content/species/data/nba_example_RLI_data_trim_marine.xlsx
+++ b/content/species/data/nba_example_RLI_data_trim_marine.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sanbiorgza.sharepoint.com/sites/RedListsquad/Shared Documents/General/NBA 2025/RLI input data/Graph input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\species\quarto\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="302" documentId="8_{8FD6900E-D1B1-4D4E-A8E6-A041C8BE9949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56612A56-BB08-42BF-A86A-8D29870DE03A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF13BE3-71A4-42DA-8531-A1E6F2C69EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{027AC6A8-209D-4E42-8E53-EE844CC37963}"/>
   </bookViews>
@@ -931,7 +931,7 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D15" sqref="D15:D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1234,7 +1234,7 @@
         <v>1</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0.98947368400000002</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1254,7 +1254,7 @@
         <v>0.78593749999998896</v>
       </c>
       <c r="D16">
-        <v>0.79687499999999301</v>
+        <v>0.78526315800000002</v>
       </c>
       <c r="E16">
         <v>0.80468749999999301</v>
@@ -2154,15 +2154,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="d08e37f2-beba-4595-a3e8-aa91f032b3fc" xsi:nil="true"/>
@@ -2173,6 +2164,15 @@
     <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2196,14 +2196,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B46C6F7B-4D94-434F-B4A8-F4B534EF89A3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23E37123-21DE-4118-A7E3-15EA5DE94433}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2213,4 +2205,12 @@
     <ds:schemaRef ds:uri="de6781d5-cbdf-44cc-b8b1-919d4413b058"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B46C6F7B-4D94-434F-B4A8-F4B534EF89A3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>